<commit_message>
Adding feature selection script
</commit_message>
<xml_diff>
--- a/Output/normality_test.xlsx
+++ b/Output/normality_test.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,6 +423,11 @@
           <t>method</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -491,6 +496,11 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>unbiased</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Overall QOL transformed Score</t>
         </is>
       </c>
     </row>

</xml_diff>